<commit_message>
test: "all" radio button functionality -> successful
</commit_message>
<xml_diff>
--- a/2025-summer/Ashley Beebakee/src/data/newsapi_crypto_dataset.xlsx
+++ b/2025-summer/Ashley Beebakee/src/data/newsapi_crypto_dataset.xlsx
@@ -12138,7 +12138,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>https://www.faz.net/aktuell/finanzen/pro-finanzen/stablecoins-gewinnen-an-bedeutung-die-veraenderung-des-geldwesens-hat-begonnen-110579243.html</t>
+          <t>https://www.faz.net/aktuell/finanzen/pro-finanzen/stablecoins-wie-sie-immer-mehr-praktische-bedeutung-erlangen-110579243.html</t>
         </is>
       </c>
       <c r="D432" t="inlineStr">
@@ -12165,7 +12165,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>https://www.faz.net/aktuell/finanzen/pro-finanzen/stablecoins-wie-sie-immer-mehr-praktische-bedeutung-erlangen-110579243.html</t>
+          <t>https://www.faz.net/aktuell/finanzen/pro-finanzen/stablecoins-gewinnen-an-bedeutung-die-veraenderung-des-geldwesens-hat-begonnen-110579243.html</t>
         </is>
       </c>
       <c r="D433" t="inlineStr">

</xml_diff>